<commit_message>
Second Commit with Modified Worksheet
</commit_message>
<xml_diff>
--- a/Worksheet.xlsx
+++ b/Worksheet.xlsx
@@ -24,12 +24,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>erw</t>
   </si>
   <si>
     <t>werw</t>
+  </si>
+  <si>
+    <t>edit</t>
   </si>
 </sst>
 </file>
@@ -347,20 +350,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3rd commit with Worksheet updated to Sherin Dua
</commit_message>
<xml_diff>
--- a/Worksheet.xlsx
+++ b/Worksheet.xlsx
@@ -24,15 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>erw</t>
+    <t>Sherin</t>
   </si>
   <si>
-    <t>werw</t>
-  </si>
-  <si>
-    <t>edit</t>
+    <t>Dua</t>
   </si>
 </sst>
 </file>
@@ -350,27 +347,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D11" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>